<commit_message>
Improve content element method handling
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8991B-4D44-104A-8550-46715BC0F3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CF058-4D0B-F148-BB11-0B7880E65F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13880" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="-500" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="818">
   <si>
     <t>Screening</t>
   </si>
@@ -2508,6 +2508,12 @@
   </si>
   <si>
     <t>TITLE: &lt;usdm:ref element="study_full_title"/&gt;&lt;br/&gt;ACRONYM: &lt;usdm:ref element="study_acronym"/&gt;</t>
+  </si>
+  <si>
+    <t>SPONSOR ID: &lt;usdm:ref element="study_identifier"/&gt;</t>
+  </si>
+  <si>
+    <t>INVALID: &lt;usdm:ref element="xxx"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2749,13 +2755,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6502,7 +6508,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6547,6 +6553,9 @@
       <c r="C3" s="6" t="s">
         <v>227</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
@@ -6554,6 +6563,9 @@
       </c>
       <c r="C4" s="6" t="s">
         <v>229</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>817</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7893,120 +7905,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>812</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="51" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="51" t="s">
         <v>709</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8098,16 +8110,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11750,6 +11762,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
@@ -11758,15 +11779,6 @@
     <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11971,6 +11983,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11983,14 +12003,6 @@
     <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Tweaks and more tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CF058-4D0B-F148-BB11-0B7880E65F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D95D49B-0333-4540-A8CD-0CD6D3B46EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-500" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="1940" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="819">
   <si>
     <t>Screening</t>
   </si>
@@ -2514,6 +2514,9 @@
   </si>
   <si>
     <t>INVALID: &lt;usdm:ref element="xxx"/&gt;</t>
+  </si>
+  <si>
+    <t>NONE:&lt;usdm:ref element="no_value_for_test"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -6508,7 +6511,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6574,6 +6577,9 @@
       </c>
       <c r="C5" s="6" t="s">
         <v>231</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>818</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tweaks to test data and fix to html handlings
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A3944A-A9A4-8B41-BAAB-1744DD661610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46DFD53-B366-9A4D-8C5F-5DBF0E1567CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="34040" windowHeight="27240" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="61700" yWindow="500" windowWidth="40340" windowHeight="27240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="823">
   <si>
     <t>Screening</t>
   </si>
@@ -2523,6 +2523,12 @@
   </si>
   <si>
     <t>IMAGE: &lt;usdm:ref image="references_test.png" type="png"/&gt;</t>
+  </si>
+  <si>
+    <t>POP: &lt;usdm:ref klass="StudyDesignPopulation" namexref="POP1" attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:ref&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The discontinuation rate associated with this oral dosing regimen was 58.6% in previous studies, and alternative clinical strategies have been sought to improve tolerance for the compound. To that end, development of a Transdermal Therapeutic System (TTS) has been initiated.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -3088,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3163,12 +3169,12 @@
       <c r="E6" s="41"/>
       <c r="F6" s="41"/>
     </row>
-    <row r="7" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="42" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>127</v>
+        <v>822</v>
       </c>
       <c r="E7" s="41"/>
       <c r="F7" s="41"/>
@@ -5250,7 +5256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -6516,8 +6522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6607,12 +6613,15 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>236</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>237</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add template processing into sections, first cut
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46DFD53-B366-9A4D-8C5F-5DBF0E1567CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE939E6-7DAC-674C-ADBF-67591D1D15CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61700" yWindow="500" windowWidth="40340" windowHeight="27240" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="61700" yWindow="500" windowWidth="40340" windowHeight="27240" firstSheet="12" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="827">
   <si>
     <t>Screening</t>
   </si>
@@ -2529,6 +2529,18 @@
   </si>
   <si>
     <t>&lt;p&gt;The discontinuation rate associated with this oral dosing regimen was 58.6% in previous studies, and alternative clinical strategies have been sought to improve tolerance for the compound. To that end, development of a Transdermal Therapeutic System (TTS) has been initiated.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:ref section="inclusion" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:ref section="exclusion" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:ref section="inclusionXXX" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:ref section="inclusion" template="xxx"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2770,13 +2782,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3094,7 +3106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E79CD3-D94C-A14B-9EDC-9C26AFA63552}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6522,8 +6534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6694,7 +6706,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>252</v>
       </c>
@@ -6703,7 +6715,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>254</v>
       </c>
@@ -6712,7 +6724,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>256</v>
       </c>
@@ -6721,7 +6733,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>258</v>
       </c>
@@ -6730,7 +6742,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>260</v>
       </c>
@@ -6739,7 +6751,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>262</v>
       </c>
@@ -6748,7 +6760,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>264</v>
       </c>
@@ -6757,7 +6769,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>266</v>
       </c>
@@ -6765,8 +6777,11 @@
       <c r="C24" s="6" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D24" s="6" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>268</v>
       </c>
@@ -6774,8 +6789,11 @@
       <c r="C25" s="6" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D25" s="6" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>270</v>
       </c>
@@ -6783,8 +6801,11 @@
       <c r="C26" s="6" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D26" s="6" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>272</v>
       </c>
@@ -6792,8 +6813,11 @@
       <c r="C27" s="6" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D27" s="6" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>274</v>
       </c>
@@ -6802,7 +6826,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>276</v>
       </c>
@@ -6811,7 +6835,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>278</v>
       </c>
@@ -6820,7 +6844,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>280</v>
       </c>
@@ -6829,7 +6853,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>282</v>
       </c>
@@ -7932,120 +7956,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="53" t="s">
         <v>812</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="51" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="51" t="s">
         <v>709</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8137,16 +8161,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11789,6 +11813,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
@@ -11797,15 +11830,6 @@
     <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12010,6 +12034,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12022,14 +12054,6 @@
     <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Improve section level 1 handling
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5F969F-6F68-8948-BF77-D67C3980ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9A18C1-BBE2-7F43-B5C9-2A8B8FE83760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="48760" yWindow="1200" windowWidth="33600" windowHeight="19460" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="829">
   <si>
     <t>Screening</t>
   </si>
@@ -2541,6 +2541,12 @@
   </si>
   <si>
     <t>&lt;usdm:ref title_page="true"/&gt;&lt;usdm:ref table_of_contents="true"/&gt;TITLE: &lt;usdm:ref element="study_full_title"/&gt;&lt;br/&gt;ACRONYM: &lt;usdm:ref element="study_acronym"/&gt;</t>
+  </si>
+  <si>
+    <t>APPendix 3</t>
+  </si>
+  <si>
+    <t>APPENDIX: Something</t>
   </si>
 </sst>
 </file>
@@ -2782,13 +2788,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6534,8 +6540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7771,9 +7777,12 @@
         <v>484</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="14" t="s">
-        <v>485</v>
+        <v>827</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -7956,120 +7965,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>812</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>709</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8161,16 +8170,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11822,17 +11831,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12033,6 +12031,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
   <ds:schemaRefs>
@@ -12042,23 +12051,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12075,4 +12067,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove m11 paths and bug fix
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E1F83-6AA4-A54E-81FD-CF3369D4DAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24DCBB5-5C14-6D4D-B095-5009D809CE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27740" yWindow="800" windowWidth="33600" windowHeight="19460" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -2510,43 +2510,43 @@
     <t>&lt;p&gt;The discontinuation rate associated with this oral dosing regimen was 58.6% in previous studies, and alternative clinical strategies have been sought to improve tolerance for the compound. To that end, development of a Transdermal Therapeutic System (TTS) has been initiated.&lt;/p&gt;</t>
   </si>
   <si>
-    <t>SECTION: &lt;usdm:ref section="exclusion" template="m11"/&gt;</t>
-  </si>
-  <si>
-    <t>SECTION: &lt;usdm:ref section="inclusionXXX" template="m11"/&gt;</t>
-  </si>
-  <si>
-    <t>SECTION: &lt;usdm:ref section="inclusion" template="xxx"/&gt;</t>
-  </si>
-  <si>
-    <t>SECTION: &lt;usdm:ref section="inclusion" template="M11"/&gt;</t>
-  </si>
-  <si>
     <t>APPendix 3</t>
   </si>
   <si>
     <t>APPENDIX: Something</t>
   </si>
   <si>
-    <t>TITLE: &lt;usdm:macro id="element" name="study_full_title"/&gt;&lt;br/&gt;ACRONYM: &lt;usdm:ref id="element" name="study_acronym"/&gt;</t>
-  </si>
-  <si>
-    <t>SPONSOR ID: &lt;usdm:ref id="element" name="study_identifier"/&gt;</t>
-  </si>
-  <si>
-    <t>INVALID: &lt;usdm:ref id="element" name="xxx"/&gt;</t>
-  </si>
-  <si>
-    <t>NONE:&lt;usdm:ref id="element" name="no_value_for_test"/&gt;</t>
-  </si>
-  <si>
-    <t>RATIONALE:&lt;usdm:ref id="element" name="study_rationale"/&gt;</t>
-  </si>
-  <si>
     <t>POP: &lt;usdm:macro id="xref" klass="StudyDesignPopulation" name="POP1" attribute="@plannedEnrollmentNumber/Range/maxValue"&gt;&lt;/usdm:ref&gt;</t>
   </si>
   <si>
-    <t>IMAGE: &lt;usdm:rmacro id="image" file="references_test.png" type="png"/&gt;</t>
+    <t>TITLE: &lt;usdm:macro id="element" name="study_full_title"/&gt;&lt;br/&gt;ACRONYM: &lt;usdm:macro id="element" name="study_acronym"/&gt;</t>
+  </si>
+  <si>
+    <t>SPONSOR ID: &lt;usdm:macro id="element" name="study_identifier"/&gt;</t>
+  </si>
+  <si>
+    <t>INVALID: &lt;usdm:macro id="element" name="xxx"/&gt;</t>
+  </si>
+  <si>
+    <t>NONE:&lt;usdm:macro id="element" name="no_value_for_test"/&gt;</t>
+  </si>
+  <si>
+    <t>RATIONALE:&lt;usdm:macro id="element" name="study_rationale"/&gt;</t>
+  </si>
+  <si>
+    <t>IMAGE: &lt;usdm:macro id="image" file="references_test.png" type="png"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:macro id="section" name="inclusion" template="M11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:macro id="section" name="exclusion" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:macro id="section" name="inclusionXXX" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>SECTION: &lt;usdm:macro id="section" name="inclusion" template="xxx"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2788,13 +2788,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6540,8 +6540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6575,7 +6575,7 @@
         <v>495</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6587,7 +6587,7 @@
         <v>227</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6598,7 +6598,7 @@
         <v>229</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6609,7 +6609,7 @@
         <v>231</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6620,7 +6620,7 @@
         <v>233</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6639,7 +6639,7 @@
         <v>237</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>827</v>
+        <v>818</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6682,7 +6682,7 @@
         <v>245</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6784,7 +6784,7 @@
         <v>267</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>819</v>
+        <v>825</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6796,7 +6796,7 @@
         <v>269</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>816</v>
+        <v>826</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6808,7 +6808,7 @@
         <v>271</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>817</v>
+        <v>827</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -6820,7 +6820,7 @@
         <v>273</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>818</v>
+        <v>828</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -7779,10 +7779,10 @@
     </row>
     <row r="134" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="14" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
@@ -7965,120 +7965,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>812</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>709</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8170,16 +8170,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11822,6 +11822,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12022,15 +12031,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12043,6 +12043,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12057,14 +12065,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
First cut SoA macro
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A889917-B0BC-9A4A-949A-9B5FB09695EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A64700-94D7-E442-8695-FE74EAD983A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="833">
   <si>
     <t>Screening</t>
   </si>
@@ -2556,6 +2556,9 @@
   </si>
   <si>
     <t>&lt;usdm:tag name="Activity1"/&gt; score of 10 to 23</t>
+  </si>
+  <si>
+    <t>SOA: &lt;usdm:macro id="section" name="soa"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2797,13 +2800,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6560,8 +6563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6705,13 +6708,16 @@
         <v>821</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>246</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="6" t="s">
         <v>247</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7985,120 +7991,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>809</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>681</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>706</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8190,16 +8196,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8211,7 +8217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1EE44-0F6C-474B-8770-DA2A14736511}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
@@ -12043,15 +12049,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
@@ -12060,6 +12057,15 @@
     <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12082,14 +12088,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -12104,4 +12102,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add footnotes to SoA
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/references.xlsx
+++ b/tests/integration_test_files/references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746A7665-7DC9-CB4F-BAA8-0BCA74E1C97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E31722-6D42-EF41-BD06-B7254AA9E17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56020" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="14" activeTab="22" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="56020" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="3" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -25,18 +25,19 @@
     <sheet name="earlyTerminationTimeline" sheetId="23" r:id="rId10"/>
     <sheet name="vsBloodPressure" sheetId="24" r:id="rId11"/>
     <sheet name="studyDesignTiming" sheetId="18" r:id="rId12"/>
-    <sheet name="studyDesignActivities" sheetId="21" r:id="rId13"/>
-    <sheet name="studyDesignInterventions" sheetId="25" r:id="rId14"/>
-    <sheet name="studyDesignIndications" sheetId="6" r:id="rId15"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId16"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId17"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId18"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId19"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId20"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId21"/>
-    <sheet name="dictionaries" sheetId="20" r:id="rId22"/>
-    <sheet name="studyDesignContent" sheetId="16" r:id="rId23"/>
-    <sheet name="configuration" sheetId="10" r:id="rId24"/>
+    <sheet name="studyDesignConditions" sheetId="26" r:id="rId13"/>
+    <sheet name="studyDesignActivities" sheetId="21" r:id="rId14"/>
+    <sheet name="studyDesignInterventions" sheetId="25" r:id="rId15"/>
+    <sheet name="studyDesignIndications" sheetId="6" r:id="rId16"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId17"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId18"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId19"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId20"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId21"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId22"/>
+    <sheet name="dictionaries" sheetId="20" r:id="rId23"/>
+    <sheet name="studyDesignContent" sheetId="16" r:id="rId24"/>
+    <sheet name="configuration" sheetId="10" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="844">
   <si>
     <t>Screening</t>
   </si>
@@ -2559,6 +2560,39 @@
   </si>
   <si>
     <t>NOTE: &lt;usdm:macro id="note" text="This is a note!"/&gt;</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>appliesTo</t>
+  </si>
+  <si>
+    <t>COND1</t>
+  </si>
+  <si>
+    <t>Hemoglobin A&lt;sup&gt;1C&lt;/sup&gt; and insulin-dependent subjects</t>
+  </si>
+  <si>
+    <t>HA1C</t>
+  </si>
+  <si>
+    <t>Performed if patient is an insulin-dependent diabetic</t>
+  </si>
+  <si>
+    <t>COND2</t>
+  </si>
+  <si>
+    <t>Questionnaire practice condition</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Practice only - It is recommended that a sampling of the CIBIC+, ADAS-Cog, DAD, and NPI-X be administered at Visit 1. Data from this sampling would not be considered as study data and would not be collected.</t>
+  </si>
+  <si>
+    <t>ADAS-Cog, CIBIC+, DAD, NPI-X</t>
   </si>
 </sst>
 </file>
@@ -2800,13 +2834,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4760,6 +4794,257 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B71E94-B17A-A74A-ACEE-31EA293881F6}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="51" style="31" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>497</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>833</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>835</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4305555-B5C2-8349-A6D3-AA57DAC0BCD5}">
   <dimension ref="A1:E37"/>
   <sheetViews>
@@ -5086,7 +5371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF1E597-6B00-4D42-8763-920CC15BFDAD}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -5300,7 +5585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FA45D-9570-C643-AC7B-6310BD62121C}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -5363,7 +5648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -5438,7 +5723,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
@@ -5850,7 +6135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5892,97 +6177,6 @@
       </c>
       <c r="H1" s="12" t="s">
         <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" style="31" customWidth="1"/>
-    <col min="6" max="6" width="24" style="20" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>740</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>737</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>741</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="31" t="s">
-        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -6055,6 +6249,97 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="24" style="20" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>741</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="31" t="s">
+        <v>736</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -6365,7 +6650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FA5DC6-70BE-E845-A085-20526138A835}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -6509,7 +6794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -6640,12 +6925,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7926,7 +8211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -8075,120 +8360,120 @@
       <c r="A1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>805</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="53" t="s">
         <v>681</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="53" t="s">
         <v>706</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8280,16 +8565,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8652,7 +8937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
@@ -11932,17 +12217,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12143,6 +12417,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12153,23 +12438,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12188,6 +12456,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
   <ds:schemaRefs>

</xml_diff>